<commit_message>
adding spreadsheet to the repo
</commit_message>
<xml_diff>
--- a/Assignments/Assignment_9/User Story Specs.xlsx
+++ b/Assignments/Assignment_9/User Story Specs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benko\Documents\GitHub\CS3398-Kree-F2019\Assignments\Assignment_9\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/this-sam-pugh/Desktop/Git_Repos/CS3398-Kree-F2019/Assignments/Assignment_9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399409B9-5C7C-443A-9854-114B223852B9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DDA1A5-2C2D-5B4C-9302-3EEF1065D73C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="17900" windowHeight="14600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Project User Stories and Functional Requirements</t>
   </si>
@@ -119,6 +119,18 @@
   </si>
   <si>
     <t>List Team Members Here: Shelby Jordan, David Kim, Sam Pugh, Ben Kowacki, Jesse Munoz</t>
+  </si>
+  <si>
+    <t>I,   I as a simplistic style user, want to utilize some buttons on the webpage instead of text input to aid in the simplicity of the webpage.</t>
+  </si>
+  <si>
+    <t>As a user, I would like to have the ability to identify my best parking option by color.</t>
+  </si>
+  <si>
+    <t>Not Here 10-10-2019</t>
+  </si>
+  <si>
+    <t>As a user looking to be able to tell apart parking garages, I would like the garages to have polygons over them where their color indicates who is allowed to park there.</t>
   </si>
 </sst>
 </file>
@@ -391,24 +403,6 @@
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -445,6 +439,24 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -831,203 +843,211 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="A8" sqref="A8:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.36328125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" customWidth="1"/>
-    <col min="3" max="3" width="16.6328125" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" customWidth="1"/>
-    <col min="6" max="6" width="15.1796875" customWidth="1"/>
+    <col min="1" max="1" width="41.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="16.81640625" customWidth="1"/>
-    <col min="10" max="10" width="49.36328125" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" customWidth="1"/>
+    <col min="10" max="10" width="49.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="10" customFormat="1" ht="55.5">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="40">
+      <c r="A1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="9" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="11" customFormat="1" ht="18" customHeight="1">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:10" s="5" customFormat="1" ht="18" customHeight="1">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="20"/>
+      <c r="E2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" s="11" customFormat="1" ht="38.5">
-      <c r="A3" s="5"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="12" t="s">
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+    </row>
+    <row r="3" spans="1:10" s="5" customFormat="1" ht="43">
+      <c r="A3" s="18"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1"/>
-      <c r="B4" s="16" t="s">
+    <row r="4" spans="1:10" ht="16">
+      <c r="A4" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="1"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1"/>
-      <c r="B6" s="16" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+    </row>
+    <row r="6" spans="1:10" ht="16">
+      <c r="A6" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="1"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="1"/>
-      <c r="B8" s="16" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="1:10" ht="37" customHeight="1">
+      <c r="A8" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="1"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="1"/>
-      <c r="B10" s="16" t="s">
+      <c r="A9" s="16"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="1:10" ht="56" customHeight="1">
+      <c r="A10" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="1"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="1"/>
-      <c r="B12" s="16" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="1:10" ht="16">
+      <c r="A12" s="16"/>
+      <c r="B12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="1"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:H2"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
adding partially done spreadsheet to repo
</commit_message>
<xml_diff>
--- a/Assignments/Assignment_9/User Story Specs.xlsx
+++ b/Assignments/Assignment_9/User Story Specs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/this-sam-pugh/Desktop/Git_Repos/CS3398-Kree-F2019/Assignments/Assignment_9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0E49CD-C90D-F740-A242-201A18BD760D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0C930E-7986-B041-8D3B-D59C3782CDF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Project User Stories and Functional Requirements</t>
   </si>
@@ -142,6 +142,11 @@
   </si>
   <si>
     <t>N-A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Awell Thught out Color Scheme to draw the user's eye to the correct location on the map
+Clickable map icons that will in turn create a submenu of options per the users choice.
+</t>
   </si>
 </sst>
 </file>
@@ -451,23 +456,23 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -854,7 +859,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -871,42 +876,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" ht="40">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
       <c r="I1" s="2"/>
       <c r="J1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="5" customFormat="1" ht="22" customHeight="1">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="21" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:10" s="5" customFormat="1" ht="16" customHeight="1">
-      <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
@@ -929,8 +934,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="66" customHeight="1">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:10" ht="207" customHeight="1">
+      <c r="A4" s="21" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -942,13 +947,15 @@
       <c r="D4" s="11">
         <v>13</v>
       </c>
-      <c r="E4" s="12"/>
+      <c r="E4" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
     </row>
     <row r="5" spans="1:10" ht="98" customHeight="1">
-      <c r="A5" s="16"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="13"/>
       <c r="C5" s="14" t="s">
         <v>23</v>
@@ -962,7 +969,7 @@
       <c r="H5" s="15"/>
     </row>
     <row r="6" spans="1:10" ht="16">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="21" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -976,7 +983,7 @@
       <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="16"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="13"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -986,7 +993,7 @@
       <c r="H7" s="15"/>
     </row>
     <row r="8" spans="1:10" ht="95" customHeight="1">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -1004,7 +1011,7 @@
       <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:10" ht="58" customHeight="1">
-      <c r="A9" s="16"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="13"/>
       <c r="C9" s="14">
         <v>34</v>
@@ -1018,7 +1025,7 @@
       <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:10" ht="109" customHeight="1">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="21" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -1036,7 +1043,7 @@
       <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:10" ht="62" customHeight="1">
-      <c r="A11" s="16"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="13"/>
       <c r="C11" s="14">
         <v>55</v>
@@ -1050,7 +1057,7 @@
       <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:10" ht="57" customHeight="1">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="21" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -1068,7 +1075,7 @@
       <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:10" ht="60" customHeight="1">
-      <c r="A13" s="16"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="13"/>
       <c r="C13" s="14">
         <v>89</v>
@@ -1083,16 +1090,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:H2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
adding sam_shelby spreadsheet info
</commit_message>
<xml_diff>
--- a/Assignments/Assignment_9/User Story Specs.xlsx
+++ b/Assignments/Assignment_9/User Story Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/this-sam-pugh/Desktop/Git_Repos/CS3398-Kree-F2019/Assignments/Assignment_9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0C930E-7986-B041-8D3B-D59C3782CDF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5538755B-AF0E-9140-B779-6D1792E7D2A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Project User Stories and Functional Requirements</t>
   </si>
@@ -144,9 +144,61 @@
     <t>N-A</t>
   </si>
   <si>
-    <t xml:space="preserve">Awell Thught out Color Scheme to draw the user's eye to the correct location on the map
-Clickable map icons that will in turn create a submenu of options per the users choice.
+    <t>A well Thught out Color Scheme to draw the user's eye to the correct location on the map
+Clickable map icons that will in turn create a submenu of options per the users choice.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactive With the google maps API and interpretted by JS controller.
+Relevent links being displayed depedning on which box or button is clicked. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iunteractivity Components and prompts to ensure click was intended before being processed. 
+Checks in the code to verifiy user input is correct. Avoid junk processing. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Any data visible to the user that could confuse them.
+Processing data showing up on the web page while processing. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A well built mapping system with easy to understand user interpretation.
+Input based off of the location one has clicked on the parking map.  
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear directions and maps based on latest campus layout and orientation. 
+Layouts that are to be updated based on Construction projects or other factors in a timely maner. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A cookie based system to help users remmember previous paths taken around campus. 
+Tie into the open street maps api to draw data from their pre built paths. </t>
+  </si>
+  <si>
+    <t>Direct people along streets without sidewalks or safe walking areas.
+Features above the minimum of what is needed to get someone from point A to point B. (Eg. Food locations, drug stores etc...)</t>
+  </si>
+  <si>
+    <t>Clearly identified areas to park and colors that most people are not colorblind to.</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>Customizable colors</t>
+  </si>
+  <si>
+    <t>The ability for a user to create a new area to park.</t>
+  </si>
+  <si>
+    <t>Interface with google api and action listeners.</t>
+  </si>
+  <si>
+    <t>A unmutable list.</t>
+  </si>
+  <si>
+    <t>Color coded list to indicate which times are more crowded with people than others.</t>
+  </si>
+  <si>
+    <t>The ability to send that list to email, facebook, or other media sharing sites.</t>
   </si>
 </sst>
 </file>
@@ -456,6 +508,9 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -470,9 +525,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -858,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -876,42 +928,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" ht="40">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
       <c r="I1" s="2"/>
       <c r="J1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="5" customFormat="1" ht="22" customHeight="1">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="20" t="s">
+      <c r="D2" s="20"/>
+      <c r="E2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:10" s="5" customFormat="1" ht="16" customHeight="1">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
@@ -934,8 +986,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="207" customHeight="1">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:10" ht="123" customHeight="1">
+      <c r="A4" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -948,14 +1000,20 @@
         <v>13</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
+        <v>32</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="98" customHeight="1">
-      <c r="A5" s="21"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="13"/>
       <c r="C5" s="14" t="s">
         <v>23</v>
@@ -963,13 +1021,21 @@
       <c r="D5" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
+      <c r="E5" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="16">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="16" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -983,7 +1049,7 @@
       <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="21"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="13"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -992,8 +1058,8 @@
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
     </row>
-    <row r="8" spans="1:10" ht="95" customHeight="1">
-      <c r="A8" s="21" t="s">
+    <row r="8" spans="1:10" ht="189" customHeight="1">
+      <c r="A8" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -1005,13 +1071,21 @@
       <c r="D8" s="11">
         <v>34</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-    </row>
-    <row r="9" spans="1:10" ht="58" customHeight="1">
-      <c r="A9" s="21"/>
+      <c r="E8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="200" customHeight="1">
+      <c r="A9" s="16"/>
       <c r="B9" s="13"/>
       <c r="C9" s="14">
         <v>34</v>
@@ -1019,13 +1093,21 @@
       <c r="D9" s="14">
         <v>34</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
+      <c r="E9" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="109" customHeight="1">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -1043,7 +1125,7 @@
       <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:10" ht="62" customHeight="1">
-      <c r="A11" s="21"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="13"/>
       <c r="C11" s="14">
         <v>55</v>
@@ -1057,7 +1139,7 @@
       <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:10" ht="57" customHeight="1">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -1075,7 +1157,7 @@
       <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:10" ht="60" customHeight="1">
-      <c r="A13" s="21"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="13"/>
       <c r="C13" s="14">
         <v>89</v>
@@ -1090,16 +1172,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:H2"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
adding shelby and sam input for user stories. Assignments 9 and 10
</commit_message>
<xml_diff>
--- a/Assignments/Assignment_9/User Story Specs.xlsx
+++ b/Assignments/Assignment_9/User Story Specs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/this-sam-pugh/Desktop/Git_Repos/CS3398-Kree-F2019/Assignments/Assignment_9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5538755B-AF0E-9140-B779-6D1792E7D2A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02E9343-5ECE-6948-B361-33107E1EBEF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15500" windowHeight="14600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -177,28 +177,36 @@
 Features above the minimum of what is needed to get someone from point A to point B. (Eg. Food locations, drug stores etc...)</t>
   </si>
   <si>
-    <t>Clearly identified areas to park and colors that most people are not colorblind to.</t>
-  </si>
-  <si>
-    <t>Legend</t>
-  </si>
-  <si>
-    <t>Customizable colors</t>
-  </si>
-  <si>
-    <t>The ability for a user to create a new area to park.</t>
-  </si>
-  <si>
-    <t>Interface with google api and action listeners.</t>
-  </si>
-  <si>
-    <t>A unmutable list.</t>
-  </si>
-  <si>
-    <t>Color coded list to indicate which times are more crowded with people than others.</t>
-  </si>
-  <si>
-    <t>The ability to send that list to email, facebook, or other media sharing sites.</t>
+    <t xml:space="preserve">(1) Clearly identified areas to park. 
+(2) Colors that most people are not colorblind to. </t>
+  </si>
+  <si>
+    <t>(1) Legend
+ (2) A contact us option.</t>
+  </si>
+  <si>
+    <t>(1) Customizable colors. 
+(2) The ability for users to update the accuracy of the predictions.</t>
+  </si>
+  <si>
+    <t>(1) The ability for a user to create a new area to park. 
+(2) The ability for users to make new walking paths.</t>
+  </si>
+  <si>
+    <t>(1) Interface with google api. 
+(2) Invisible interface on the map that has action listeners.</t>
+  </si>
+  <si>
+    <t>(1) A unmutable list. 
+(2) The mouse should change from a pointer to a hand.</t>
+  </si>
+  <si>
+    <t>(1) Color coded list to indicate which times are more crowded with people than others.
+ (2) Traffic indicators near parking areas.</t>
+  </si>
+  <si>
+    <t>(1) The ability to send that list to email, facebook, or other media sharing sites. 
+(2) The ablilty to change any output.</t>
   </si>
 </sst>
 </file>
@@ -496,35 +504,35 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -910,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -928,42 +936,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" ht="40">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
       <c r="I1" s="2"/>
       <c r="J1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="5" customFormat="1" ht="22" customHeight="1">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="21" t="s">
+      <c r="D2" s="17"/>
+      <c r="E2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:10" s="5" customFormat="1" ht="16" customHeight="1">
-      <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
@@ -986,8 +994,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="123" customHeight="1">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:10" ht="103" customHeight="1">
+      <c r="A4" s="19" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -999,43 +1007,43 @@
       <c r="D4" s="11">
         <v>13</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="98" customHeight="1">
-      <c r="A5" s="16"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14" t="s">
+    <row r="5" spans="1:10" ht="183" customHeight="1">
+      <c r="A5" s="19"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="20" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="16">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="19" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -1043,23 +1051,23 @@
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="16"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
     </row>
     <row r="8" spans="1:10" ht="189" customHeight="1">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -1071,43 +1079,43 @@
       <c r="D8" s="11">
         <v>34</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="200" customHeight="1">
-      <c r="A9" s="16"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14">
+      <c r="A9" s="19"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13">
         <v>34</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="13">
         <v>34</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="H9" s="20" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="109" customHeight="1">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="19" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -1119,27 +1127,27 @@
       <c r="D10" s="11">
         <v>34</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
     </row>
     <row r="11" spans="1:10" ht="62" customHeight="1">
-      <c r="A11" s="16"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14">
+      <c r="A11" s="19"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="13">
         <v>55</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="13">
         <v>55</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
     </row>
     <row r="12" spans="1:10" ht="57" customHeight="1">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="19" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -1151,37 +1159,37 @@
       <c r="D12" s="11">
         <v>13</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
     </row>
     <row r="13" spans="1:10" ht="60" customHeight="1">
-      <c r="A13" s="16"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="14">
+      <c r="A13" s="19"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13">
         <v>89</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="13">
         <v>55</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:H2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Added must/should/could/won't to Ben
</commit_message>
<xml_diff>
--- a/Assignments/Assignment_9/User Story Specs.xlsx
+++ b/Assignments/Assignment_9/User Story Specs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jessem1020\Documents\GitHub\CS3398-Kree-F2019\Assignments\Assignment_9\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BenVR\Documents\GitHub\CS3398-Kree-F2019\Assignments\Assignment_9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714E50E0-797B-4639-91C6-5BB4B0D323A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD611E99-C948-437F-A631-EDB60B5080FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32811" yWindow="1457" windowWidth="27635" windowHeight="15034" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>Project User Stories and Functional Requirements</t>
   </si>
@@ -231,6 +231,38 @@
   </si>
   <si>
     <t>1) A way to reserve a parking spot.                                                                                                                                                                                                                                                                                                                                     2) A way to see spots for future times.</t>
+  </si>
+  <si>
+    <t>Clean looking, square polygons.
+Way to tell garages apart from lots.</t>
+  </si>
+  <si>
+    <t>Every garage/lot accounted for with its color reflecting which permit is allowed to park there.
+Accurate shapes and sizes.</t>
+  </si>
+  <si>
+    <t>Capacity based on type of vehicle visible when user clicks on the polygon.
+Option to hide certain classes of lots.</t>
+  </si>
+  <si>
+    <t>Way to concatenate paths. 
+Easily-visible and smooth path between points.</t>
+  </si>
+  <si>
+    <t>Way to select one point and one polygon and get directions between them. 
+Way to generate path based on user input or selection.</t>
+  </si>
+  <si>
+    <t>Feature to automatically select a path based on time/traffic, not just shortest distance. 
+Ability to add path between apartment complex or unlisted parking space and campus.</t>
+  </si>
+  <si>
+    <t>Real-time capacity or estimate.
+Way for users to move around polygons or add custom polygons.</t>
+  </si>
+  <si>
+    <t>Default Google pathfinding.
+Invalid or out-of-date paths.</t>
   </si>
 </sst>
 </file>
@@ -540,6 +572,9 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -554,9 +589,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -942,60 +974,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="41.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="1" max="1" width="41.3046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.4609375" customWidth="1"/>
+    <col min="3" max="3" width="16.69140625" customWidth="1"/>
+    <col min="4" max="4" width="13.4609375" customWidth="1"/>
+    <col min="5" max="5" width="15.4609375" customWidth="1"/>
+    <col min="6" max="6" width="15.07421875" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="16.77734375" customWidth="1"/>
-    <col min="10" max="10" width="49.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.765625" customWidth="1"/>
+    <col min="10" max="10" width="49.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" ht="54">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="55.3">
+      <c r="A1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
       <c r="I1" s="2"/>
       <c r="J1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="5" customFormat="1" ht="22.05" customHeight="1">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:10" s="5" customFormat="1" ht="22.1" customHeight="1">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="20" t="s">
+      <c r="D2" s="20"/>
+      <c r="E2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
     </row>
-    <row r="3" spans="1:10" s="5" customFormat="1" ht="16.05" customHeight="1">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18"/>
+    <row r="3" spans="1:10" s="5" customFormat="1" ht="16.100000000000001" customHeight="1">
+      <c r="A3" s="18"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
@@ -1018,8 +1050,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="103.05" customHeight="1">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:10" ht="103.1" customHeight="1">
+      <c r="A4" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -1045,7 +1077,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="183" customHeight="1">
-      <c r="A5" s="21"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="12"/>
       <c r="C5" s="13" t="s">
         <v>23</v>
@@ -1067,7 +1099,7 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="16" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -1081,7 +1113,7 @@
       <c r="H6" s="15"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="21"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="12"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -1091,7 +1123,7 @@
       <c r="H7" s="14"/>
     </row>
     <row r="8" spans="1:10" ht="189" customHeight="1">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -1117,7 +1149,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="199.95" customHeight="1">
-      <c r="A9" s="21"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="12"/>
       <c r="C9" s="13">
         <v>34</v>
@@ -1138,8 +1170,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="109.05" customHeight="1">
-      <c r="A10" s="21" t="s">
+    <row r="10" spans="1:10" ht="131.15">
+      <c r="A10" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -1151,13 +1183,21 @@
       <c r="D10" s="11">
         <v>34</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
+      <c r="E10" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" ht="61.95" customHeight="1">
-      <c r="A11" s="21"/>
+    <row r="11" spans="1:10" ht="160.30000000000001">
+      <c r="A11" s="16"/>
       <c r="B11" s="12"/>
       <c r="C11" s="13">
         <v>55</v>
@@ -1165,13 +1205,21 @@
       <c r="D11" s="13">
         <v>55</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
+      <c r="E11" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="181.2" customHeight="1">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -1196,8 +1244,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="223.8" customHeight="1">
-      <c r="A13" s="21"/>
+    <row r="13" spans="1:10" ht="223.85" customHeight="1">
+      <c r="A13" s="16"/>
       <c r="B13" s="12"/>
       <c r="C13" s="13">
         <v>89</v>
@@ -1220,16 +1268,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:H2"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>